<commit_message>
update of supplemental tables
</commit_message>
<xml_diff>
--- a/Table_S1.xlsx
+++ b/Table_S1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrw657\Documents\Projects\Whitehall\SUBMISSION_XXJULY2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vrw657\Documents\Projects\Whitehall\RESUBMISSION_XXAUG2021_JCEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -335,44 +335,23 @@
     <t>Fully adjusted model**</t>
   </si>
   <si>
-    <t>Table S1. All marginal and time interaction estimates from the GEE models (N=8,182).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">*covariates: organizational justice, organization justice </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>×</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> time, age at baseline, sex, ethnicity, educational level, job grade, income
-**covariates: base model covariates + alcohol consumption, smoking status, exercise, diabetes status, fasting status, medication use
+    <t>ln(fasting insulin) (ln(µIU/mL))</t>
+  </si>
+  <si>
+    <t>Table S1. Marginal and time interaction estimates from the GEE models (N=8,182).</t>
+  </si>
+  <si>
+    <t>* covariates: organizational justice × time, age at baseline, sex, ethnicity, educational level, job grade, income
+** covariates: base model covariates + marital status, alcohol consumption, smoking status, exercise, diabetes status, presence of any longstanding illness, fasting status, medication use
 The estimates are presented with 95% confidence intervals.
 Abbreviations: BMI – body mass index; DBP – diastolic blood pressure; HDL-C – high-density lipoprotein cholesterol; LDL-C – low-density lipoprotein cholesterol; SBP – systolic blood pressure; TC – total cholesterol</t>
-    </r>
-  </si>
-  <si>
-    <t>ln(fasting insulin) (ln(µIU/mL))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -396,12 +375,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -411,7 +384,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -435,20 +408,54 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
       <top style="hair">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="hair">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -456,16 +463,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -777,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,64 +804,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="A1" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="8"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -860,7 +872,7 @@
       <c r="B5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -880,7 +892,7 @@
       <c r="B6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>64</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -900,7 +912,7 @@
       <c r="B7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>66</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -918,9 +930,9 @@
         <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -940,7 +952,7 @@
       <c r="B9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -960,7 +972,7 @@
       <c r="B10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -980,7 +992,7 @@
       <c r="B11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -1000,7 +1012,7 @@
       <c r="B12" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>75</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -1020,7 +1032,7 @@
       <c r="B13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>77</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -1040,7 +1052,7 @@
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>78</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -1060,7 +1072,7 @@
       <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -1080,7 +1092,7 @@
       <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>82</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -1138,7 +1150,7 @@
         <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>25</v>
@@ -1254,34 +1266,34 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
+    <row r="26" spans="1:6" ht="98.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
   </sheetData>
   <sortState ref="A2:D320">

</xml_diff>